<commit_message>
added link to website
</commit_message>
<xml_diff>
--- a/eRCaGuy_analogReadXXbit Library Speed Calcs - Gabriel.xlsx
+++ b/eRCaGuy_analogReadXXbit Library Speed Calcs - Gabriel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Resolution</t>
   </si>
@@ -602,6 +602,12 @@
       </rPr>
       <t>*1000</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Library webpage: </t>
+  </si>
+  <si>
+    <t>http://electricrcaircraftguy.blogspot.com/2014/05/using-arduino-unos-built-in-16-bit-adc.html</t>
   </si>
 </sst>
 </file>
@@ -614,7 +620,7 @@
     <numFmt numFmtId="166" formatCode="0.000\ &quot;Hz&quot;"/>
     <numFmt numFmtId="167" formatCode="0.0000\ &quot;Hz&quot;"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -804,6 +810,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1034,7 +1048,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1128,6 +1142,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1143,9 +1160,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1718,8 +1736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:AE24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1736,19 +1754,26 @@
     <col min="11" max="11" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:31" ht="15.75" thickBot="1"/>
+    <row r="1" spans="2:31" ht="15.75" thickBot="1">
+      <c r="C1" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="62" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="2" spans="2:31" ht="55.5" customHeight="1" thickBot="1">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58"/>
       <c r="K2" s="26"/>
       <c r="N2" t="s">
         <v>8</v>
@@ -1776,7 +1801,7 @@
       <c r="I3" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="58" t="s">
+      <c r="J3" s="59" t="s">
         <v>21</v>
       </c>
       <c r="K3" s="8"/>
@@ -1788,7 +1813,7 @@
       <c r="B4" s="7"/>
       <c r="C4" s="20"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="55" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="8"/>
@@ -1796,7 +1821,7 @@
         <v>4</v>
       </c>
       <c r="I4" s="34"/>
-      <c r="J4" s="59"/>
+      <c r="J4" s="60"/>
       <c r="K4" s="8"/>
       <c r="P4" s="24" t="s">
         <v>12</v>
@@ -2564,10 +2589,11 @@
     <hyperlink ref="C23" r:id="rId4"/>
     <hyperlink ref="G24" r:id="rId5"/>
     <hyperlink ref="E20" r:id="rId6"/>
+    <hyperlink ref="D1" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
-  <drawing r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
+  <drawing r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>